<commit_message>
Symal Bulleen rapid build
</commit_message>
<xml_diff>
--- a/Symal/23346/NEL-CNT-SDC-2990-PQA-ITP-0016.00.IFU.00.01_RES.xlsx
+++ b/Symal/23346/NEL-CNT-SDC-2990-PQA-ITP-0016.00.IFU.00.01_RES.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\William\Desktop\CONQA\_Git\CONQA\Symal\23346\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E61D934-BCCA-4EE9-A33E-DB398B1A58F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB5B76E-1B72-465F-86C2-616EE4AE5172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7365" yWindow="120" windowWidth="28830" windowHeight="20385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4290" yWindow="1215" windowWidth="28830" windowHeight="20385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="res" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">res!$A$1:$L$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">res!$A$1:$I$282</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="144">
   <si>
     <t>type</t>
   </si>
@@ -70,37 +70,391 @@
     <t>1.0 Preliminaries (Include all aspects of Materials, Approvals, IFC Drawings, etc. Ensure all required permits have been raised prior to commencing works)</t>
   </si>
   <si>
-    <t xml:space="preserve">1.1 - </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resp. Person - </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Specification Reference - </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acceptance Criteria - </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Method - </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Frequency - </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inspection/Verification (Name, signature &amp; date): Spark NEL Engineer - </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inspection/Verification (Name, signature &amp; date): Sub-Contractor - </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inspection/Verification (Name, signature &amp; date): Nominated Authority - </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inspection/Verification (Name, signature &amp; date): IREA - </t>
-  </si>
-  <si>
     <t xml:space="preserve">Records/Documents - </t>
+  </si>
+  <si>
+    <t>2.0 Operations (Include Work Execution – Installation / Manufacturing Process step-by-step)</t>
+  </si>
+  <si>
+    <t>3.0 Post Operations (Include Inspection and Testing)</t>
+  </si>
+  <si>
+    <t>4.0 Quality</t>
+  </si>
+  <si>
+    <t>1.1 - Construction Package Approval</t>
+  </si>
+  <si>
+    <t>Resp. Person - PE</t>
+  </si>
+  <si>
+    <t>Specification Reference - PSDR Part F6 2 (a) to (h)</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria - Construction Documentation shall be submitted and approved prior to commencing work at site.</t>
+  </si>
+  <si>
+    <t>Test Method - R</t>
+  </si>
+  <si>
+    <t>Test Frequency - PW</t>
+  </si>
+  <si>
+    <t>Inspection/Verification (Name, signature &amp; date): Sub-Contractor - NR</t>
+  </si>
+  <si>
+    <t>Inspection/Verification (Name, signature &amp; date): Spark NEL Engineer - HP</t>
+  </si>
+  <si>
+    <t>Inspection/Verification (Name, signature &amp; date): Nominated Authority - NR</t>
+  </si>
+  <si>
+    <t>Inspection/Verification (Name, signature &amp; date): IREA - NR</t>
+  </si>
+  <si>
+    <t>Records/Documents - IFU Construction Package</t>
+  </si>
+  <si>
+    <t>textbox</t>
+  </si>
+  <si>
+    <t>holdpoint</t>
+  </si>
+  <si>
+    <t>AUTHORITY HOLDPOINT</t>
+  </si>
+  <si>
+    <t>• InEight Reference: #</t>
+  </si>
+  <si>
+    <t>1.2 - Design status</t>
+  </si>
+  <si>
+    <t>Specification Reference - PSDR Part F5, 2(b) &amp; (c)(i)</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria - Design to be IFC prior to works commencing</t>
+  </si>
+  <si>
+    <t>Test Method - V</t>
+  </si>
+  <si>
+    <t>Records/Documents - IFC Drawings</t>
+  </si>
+  <si>
+    <t>Resp. Person - SE</t>
+  </si>
+  <si>
+    <t>1.3 - All Equipment calibrated</t>
+  </si>
+  <si>
+    <t>Specification Reference - Quality Management Plan Section 11.1</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria - Equipment calibration certificates filed in InEight</t>
+  </si>
+  <si>
+    <t>• Ensure all equipment associated with the relevant works is calibrated</t>
+  </si>
+  <si>
+    <t>Inspection/Verification (Name, signature &amp; date): Sub-Contractor - HP</t>
+  </si>
+  <si>
+    <t>Records/Documents - Calibration Certificates</t>
+  </si>
+  <si>
+    <t>1.4 - Premixed Concrete</t>
+  </si>
+  <si>
+    <t>Specification Reference - Vic Roads 703.05, Table 703.111 IFC Drawings</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria - Premixed concrete conforms with requirements of AS1379, 703.05 and Table 703.111</t>
+  </si>
+  <si>
+    <t>Records/Documents - Delivery Docket</t>
+  </si>
+  <si>
+    <t>1.5 - Survey Set Out</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria - Clearly mark limit of works; Chainage, offsets, cut/fill level etc. (if required)</t>
+  </si>
+  <si>
+    <t>Specification Reference - PSDR Part F4 Section 6 IFC Drawings, VicRoads 703.17 IFC Drawings</t>
+  </si>
+  <si>
+    <t>Inspection/Verification (Name, signature &amp; date): Nominated Authority - HP</t>
+  </si>
+  <si>
+    <t>Inspection/Verification (Name, signature &amp; date): IREA - WP</t>
+  </si>
+  <si>
+    <t>• HP Release InEight Reference: #</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Survey Record InEight Reference: </t>
+  </si>
+  <si>
+    <t>2.1 - Excavations and bedding preparation</t>
+  </si>
+  <si>
+    <t>Specification Reference - VicRoads 703.20, 703.21 IFC Drawings</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria - Excavation not to extend more than 150mm from the adjacent face of existing pavement.</t>
+  </si>
+  <si>
+    <t>• Bedding material shall be compacted size 20mm Class 3 or Class 4 Crushed Rock to 98% standards compaction unless shown otherwise on the drawings Material properties, testing and testing frequency shall be in accordance with section 812</t>
+  </si>
+  <si>
+    <t>Test Frequency - PL</t>
+  </si>
+  <si>
+    <t>Inspection/Verification (Name, signature &amp; date): Sub-Contractor - WP</t>
+  </si>
+  <si>
+    <t>Inspection/Verification (Name, signature &amp; date): Spark NEL Engineer - WP</t>
+  </si>
+  <si>
+    <t>Records/Documents - Material delivery dockets</t>
+  </si>
+  <si>
+    <t>2.2 - Machine Extrusion</t>
+  </si>
+  <si>
+    <t>• Traffic Routes – a minimum of, or equivalent to, 320 kg of cementitious material or geopolymer binder per cubic metre of concrete</t>
+  </si>
+  <si>
+    <t>• Surfaces shall be substantially free from surface pitting larger than 5mm diameter</t>
+  </si>
+  <si>
+    <t>• Local Streets – a minimum of, or equivalent to, 280 kg of cementitious material or geopolymer binder per cubic metre of concrete</t>
+  </si>
+  <si>
+    <t>○ Concrete used in kerb extrusion machines will not be subject to compressive strength requirements but shall have a minimum cementitious material content in the finished concrete as follows:</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria - Concrete shall be fed to the machine at a uniform rate. The machine shall be operated to produce a satisfactorily compacted, dense mass of concrete free of any faulty or honeycombed patches.</t>
+  </si>
+  <si>
+    <t>Specification Reference - VicRoads 703.05(b) 703.23 IFC Drawings</t>
+  </si>
+  <si>
+    <t>Records/Documents - Concrete delivery dockets</t>
+  </si>
+  <si>
+    <t>2.3 - Profile transitions and matching existing sections</t>
+  </si>
+  <si>
+    <t>Specification Reference - VicRoads 703.24 IFC Drawings</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria - Change of profile shall be made at a constant rate between 10 and 20mm per metre. Transitions between different profiles shall be made in accordance with the drawings</t>
+  </si>
+  <si>
+    <t>Records/Documents - This ITP</t>
+  </si>
+  <si>
+    <t>2.4 - Surface Finish</t>
+  </si>
+  <si>
+    <t>Specification Reference - VicRoads 703.25 AS3610 IFC Drawings</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria - All edgings shall be rendered and have a steel trowel finish. Rendering shall be applied within 30 minutes of placing or extruding concrete.</t>
+  </si>
+  <si>
+    <t>• Permanently hidden concrete surfaces of edgings shall have a Class 4 surface finish in accordance with AS3610.</t>
+  </si>
+  <si>
+    <t>2.5 - Joints</t>
+  </si>
+  <si>
+    <t>Specification Reference - VicRoads 703.26 IFC Drawings</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria - Transverse joints shall be constructed at regular intervals not exceeding 2.5m.</t>
+  </si>
+  <si>
+    <t>• Expansion joints shall be placed at junctions with bridges, and shall be 15 mm wide and filled with cork or bituminous impregnated particle board strip extending for the full width and full depth of the edging.</t>
+  </si>
+  <si>
+    <t>• Expansion joint and control joints as per details shown on the IFC drawings.</t>
+  </si>
+  <si>
+    <t>2.6 - Marking Conduit positions</t>
+  </si>
+  <si>
+    <t>Specification Reference - VicRoads 703.28</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria - Existing conduits passing under edgings shall be marked by a chase in the edge immediately above the conduit together with a suitable identification mark.</t>
+  </si>
+  <si>
+    <t>Records/Documents - This ITP, Photos</t>
+  </si>
+  <si>
+    <t>2.7 - Curing and Protection of concrete</t>
+  </si>
+  <si>
+    <t>Specification Reference - VicRoads 703.10, 703.27 AS 3799 IFC drawings</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria - Exposed concrete surfaces to be cured Immediately after finishing operations with either water, wet hessian or curing compound complying with AS 3799 for a minimum period of 7 days.</t>
+  </si>
+  <si>
+    <t>• Exceptions are edges which require a minimum period of 3 days curing</t>
+  </si>
+  <si>
+    <t>• All concrete shall be protected from early loading</t>
+  </si>
+  <si>
+    <t>2.8 - Inspection of Concrete Surface</t>
+  </si>
+  <si>
+    <t>Specification Reference - VicRoads 703.25, 703.26 IFC drawings</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria - After finishing, all work shall present a consistently neat appearance of uniform colour.   All edges shall be sharp and clean and bullnoses shall be regular and of uniform radius.</t>
+  </si>
+  <si>
+    <t>• Surface finish and joints to comply with 703.25 and 703.26. The concrete shall have no surface cracks at any stage after construction of width greater than 0.2mm</t>
+  </si>
+  <si>
+    <t>2.9 - Backfill and restoration</t>
+  </si>
+  <si>
+    <t>Specification Reference - Vic Roads 703.29 IFC drawings</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria - Backfill to be placed once concrete has cured for at least 3 days as per drawings.</t>
+  </si>
+  <si>
+    <t>• Fill to be placed and compacted in layers not exceeding 150mm to a width not less than 300mm behind the edging to the top of the edging</t>
+  </si>
+  <si>
+    <t>Resp. Person - SE / QSR</t>
+  </si>
+  <si>
+    <t>2.10 - Crack of Concrete</t>
+  </si>
+  <si>
+    <t>Specification Reference - VR 703.30 (a) (b) (c)</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria - The concrete shall have no surface cracks at any stage after construction of width greater than 0.2mm.</t>
+  </si>
+  <si>
+    <t>• Cracked sections of concrete shall be either removed and replaced, or repaired in accordance with Section 687, as directed by the Superintendent.</t>
+  </si>
+  <si>
+    <t>Inspection/Verification (Name, signature &amp; date): Nominated Authority - WP</t>
+  </si>
+  <si>
+    <t>3.1 - As-Builts Survey</t>
+  </si>
+  <si>
+    <t>Specification Reference - VicRoads 703.15 IFC Drawings</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria - Ensure As-Built survey is compared within the required tolerance to Design specification.</t>
+  </si>
+  <si>
+    <t>• All concrete paving shall be shaped to match existing fixtures e.g. pit covers, edging and VC withing 5 mm</t>
+  </si>
+  <si>
+    <t>• The departure of the finished work from line or level shall not exceed 10 mm at any point and rate of deviation shall not exceed 10mm in 10m, except on curve the deviation shall not exceed 5mm at any point.</t>
+  </si>
+  <si>
+    <t>• Section dimensions shall not differ from those in the drawings by more than 5mm.</t>
+  </si>
+  <si>
+    <t>• Ensure all locations and work area highlighted as per Construction Lot in Work Lot Map.</t>
+  </si>
+  <si>
+    <t>Test Method - I &amp; V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Records/Documents - As-Built Survey Report </t>
+  </si>
+  <si>
+    <t>• Work Lot Map</t>
+  </si>
+  <si>
+    <t>3.2 - Final Inspection Site Walk</t>
+  </si>
+  <si>
+    <t>Specification Reference - CQMP Section 12</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria - Ensure at the end of each work conducted that Quality Control conduct an Inspection walk with Engineer to identify potential defects.</t>
+  </si>
+  <si>
+    <t>Records/Documents - Punch List Record</t>
+  </si>
+  <si>
+    <t>3.3 - Redline Drawings</t>
+  </si>
+  <si>
+    <t>Specification Reference - Design Management PlanNEL-CNT- SDC-2990-PDM- MPL-0001 Section 5.4</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria - Redline Drawings submitted to Project for creation of As- Built Drawings.</t>
+  </si>
+  <si>
+    <t>Records/Documents - Red-Line Marked Up IFC Drawing(s)</t>
+  </si>
+  <si>
+    <t>3.4 - Verification and Lot Records complete</t>
+  </si>
+  <si>
+    <t>Specification Reference - CQMP Section 8.3</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria - Progressive monitoring and signoff of Checklists occurs, and test records are collected. Ensure completed work checklists, inspection and test results and Subcontractor conformance records are progressively and permanently saved and stored as soon as possible after they are received.</t>
+  </si>
+  <si>
+    <t>• Completed construction lot records are transferred to the project Quality Team for final record verification prior to being closed</t>
+  </si>
+  <si>
+    <t>Records/Documents - Lot Record Lot Map</t>
+  </si>
+  <si>
+    <t>3.5 - NCR Close out (if applicable)</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria - All NCR’s presented for closure</t>
+  </si>
+  <si>
+    <t>Records/Documents -</t>
+  </si>
+  <si>
+    <t>• NCR Module</t>
+  </si>
+  <si>
+    <t>• NCR InEight Reference: #</t>
+  </si>
+  <si>
+    <t>4.1 - Identification and control of non- conforming products or services (if applicable)</t>
+  </si>
+  <si>
+    <t>Resp. Person - QSR</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria - Review and confirm closure of NCR’s and associated RFI’s prior to closing of construction lot</t>
+  </si>
+  <si>
+    <t>Records/Documents - NCR closed with related documentation</t>
+  </si>
+  <si>
+    <t>4.2 - Check all quality records for lot closure</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria - All applicable quality records are complete</t>
+  </si>
+  <si>
+    <t>Records/Documents - Compiled documents (all data reports and records)</t>
   </si>
 </sst>
 </file>
@@ -243,7 +597,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -439,6 +793,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -600,12 +960,19 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -961,16 +1328,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I14"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:I282"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B3" sqref="B3:B264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="174" style="1" customWidth="1"/>
+    <col min="2" max="2" width="209.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" style="1" customWidth="1"/>
     <col min="4" max="7" width="9.140625" style="1"/>
     <col min="8" max="8" width="53.85546875" style="1" customWidth="1"/>
@@ -1030,95 +1398,2247 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1" t="s">
+    <row r="67" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B70" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="1" t="s">
+    <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B121" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B134" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B145" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B149" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B150" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B158" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A170" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B170" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A171" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A172" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A173" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A174" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A175" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A176" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A177" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A178" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A179" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A180" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A181" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A182" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B182" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A183" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A184" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A185" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A186" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A187" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A188" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A189" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A190" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A191" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A192" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A194" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B194" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B195" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
+    <row r="196" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A196" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B196" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A197" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A198" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A199" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A200" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A201" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A202" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A203" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A204" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A205" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A206" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A207" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A208" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A209" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A210" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A211" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A212" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A213" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B213" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A214" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A215" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A216" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B216" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A217" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A218" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A219" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A220" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A221" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A222" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A223" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A224" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B224" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A225" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A226" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A227" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A228" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A229" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A230" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A231" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A232" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B232" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A233" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B233" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A234" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B234" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A235" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B235" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A236" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B236" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A237" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B237" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A238" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B238" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A239" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B239" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A240" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A241" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A242" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B242" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A243" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A244" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B244" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A245" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B245" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A246" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A247" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A248" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B248" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A249" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B249" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A250" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B250" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A251" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B251" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A252" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B252" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A253" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B253" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A254" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B254" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A255" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B255" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A256" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B256" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A257" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B257" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A258" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B258" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A259" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B259" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A260" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B260" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A261" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B261" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A262" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B262" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A263" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B263" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A264" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B264" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="1" t="s">
+    <row r="265" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A265" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B265" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A266" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B266" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A267" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B267" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A268" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B268" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A269" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B269" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>25</v>
+    <row r="270" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A270" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B270" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A271" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B271" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A272" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B272" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A273" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B273" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A274" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B274" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A275" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B275" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A276" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B276" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A277" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B277" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A278" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B278" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A279" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B279" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A280" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B280" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A281" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B281" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A282" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B282" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I282" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="checklist"/>
+        <filter val="section"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>